<commit_message>
got bubble working correctly
</commit_message>
<xml_diff>
--- a/Report_5558.xlsx
+++ b/Report_5558.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Report_5558.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,15 +24,6 @@
     <t>Your firm</t>
   </si>
   <si>
-    <t>Total: All Businesses</t>
-  </si>
-  <si>
-    <t>Occupancy Rate: Leaders</t>
-  </si>
-  <si>
-    <t>Occupancy Rate: Laggers</t>
-  </si>
-  <si>
     <t>PROFITABILITY ANALYSIS</t>
   </si>
   <si>
@@ -334,6 +325,15 @@
   </si>
   <si>
     <t>International</t>
+  </si>
+  <si>
+    <t>Total - All Businesses</t>
+  </si>
+  <si>
+    <t>Occupancy Rate - Leaders</t>
+  </si>
+  <si>
+    <t>Occupancy Rate - Laggers</t>
   </si>
 </sst>
 </file>
@@ -344,10 +344,26 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,8 +386,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -379,7 +399,11 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -709,37 +733,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E146"/>
+  <dimension ref="A2:K145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:11">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
         <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>0.78749999999999998</v>
@@ -751,9 +781,9 @@
         <v>0.76970000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>4.7899999999999998E-2</v>
@@ -765,9 +795,9 @@
         <v>9.5699999999999993E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>0.1043</v>
@@ -779,9 +809,9 @@
         <v>7.85E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>6.0299999999999999E-2</v>
@@ -793,486 +823,498 @@
         <v>5.6099999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.3735</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.2399</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.46989999999999998</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2">
+        <v>7159584</v>
+      </c>
+      <c r="J8" s="2">
+        <v>8528913</v>
+      </c>
+      <c r="K8" s="2">
+        <v>10283110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.62649999999999995</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.7601</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.53010000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2">
-        <v>7159584</v>
-      </c>
-      <c r="D8" s="2">
-        <v>8528913</v>
-      </c>
-      <c r="E8" s="2">
-        <v>10283110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.3735</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.2399</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.46989999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="C11" s="1">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.62649999999999995</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.7601</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.53010000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="C12" s="1">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="C13" s="1">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.55E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1">
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4.1999999999999997E-3</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1.8E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="C14" s="1">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1.17E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1">
-        <v>3.7000000000000002E-3</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1.6999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="C15" s="1">
+        <v>8.5400000000000004E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3.7699999999999997E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.16289999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1">
-        <v>1.1299999999999999E-2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1.55E-2</v>
-      </c>
-      <c r="E14" s="1">
-        <v>6.8999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1.8700000000000001E-2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1.1900000000000001E-2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1.17E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
       <c r="C16" s="1">
-        <v>8.5400000000000004E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="D16" s="1">
-        <v>3.7699999999999997E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>0.16289999999999999</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>2.2200000000000001E-2</v>
       </c>
       <c r="D17" s="1">
-        <v>1.7600000000000001E-2</v>
+        <v>3.8E-3</v>
       </c>
       <c r="E17" s="1">
-        <v>4.3E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1">
-        <v>2.2200000000000001E-2</v>
+        <v>6.9800000000000001E-2</v>
       </c>
       <c r="D18" s="1">
-        <v>3.8E-3</v>
+        <v>4.99E-2</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>7.4499999999999997E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1">
-        <v>6.9800000000000001E-2</v>
+        <v>4.8099999999999997E-2</v>
       </c>
       <c r="D19" s="1">
-        <v>4.99E-2</v>
+        <v>8.0999999999999996E-3</v>
       </c>
       <c r="E19" s="1">
-        <v>7.4499999999999997E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1">
-        <v>4.8099999999999997E-2</v>
+        <v>3.3799999999999997E-2</v>
       </c>
       <c r="D20" s="1">
-        <v>8.0999999999999996E-3</v>
+        <v>2.3300000000000001E-2</v>
       </c>
       <c r="E20" s="1">
-        <v>8.8000000000000005E-3</v>
+        <v>3.2500000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1">
-        <v>3.3799999999999997E-2</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="D21" s="1">
-        <v>2.3300000000000001E-2</v>
+        <v>1.12E-2</v>
       </c>
       <c r="E21" s="1">
-        <v>3.2500000000000001E-2</v>
+        <v>6.3E-3</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1">
-        <v>8.2000000000000007E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D22" s="1">
-        <v>1.12E-2</v>
+        <v>1.72E-2</v>
       </c>
       <c r="E22" s="1">
-        <v>6.3E-3</v>
+        <v>5.7000000000000002E-3</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>1.6899999999999998E-2</v>
       </c>
       <c r="D23" s="1">
-        <v>1.72E-2</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="E23" s="1">
-        <v>5.7000000000000002E-3</v>
+        <v>5.8999999999999999E-3</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1">
-        <v>1.6899999999999998E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D24" s="1">
-        <v>4.4999999999999997E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="E24" s="1">
-        <v>5.8999999999999999E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="D25" s="1">
-        <v>1.6000000000000001E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E25" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1">
-        <v>3.0999999999999999E-3</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="D26" s="1">
-        <v>8.0000000000000004E-4</v>
+        <v>0.14810000000000001</v>
       </c>
       <c r="E26" s="1">
-        <v>1.1999999999999999E-3</v>
+        <v>1.1299999999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>3.2399999999999998E-2</v>
       </c>
       <c r="D27" s="1">
-        <v>0.14810000000000001</v>
+        <v>2.9399999999999999E-2</v>
       </c>
       <c r="E27" s="1">
-        <v>1.1299999999999999E-2</v>
+        <v>3.2800000000000003E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1">
-        <v>3.2399999999999998E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
       <c r="D28" s="1">
-        <v>2.9399999999999999E-2</v>
+        <v>0.1017</v>
       </c>
       <c r="E28" s="1">
-        <v>3.2800000000000003E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1">
-        <v>8.4400000000000003E-2</v>
+        <v>0.5534</v>
       </c>
       <c r="D29" s="1">
-        <v>0.1017</v>
+        <v>0.48759999999999998</v>
       </c>
       <c r="E29" s="1">
-        <v>0.08</v>
+        <v>0.45329999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0.5534</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0.48759999999999998</v>
-      </c>
-      <c r="E30" s="1">
-        <v>0.45329999999999998</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>2.61</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>2.67</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32">
-        <v>2.61</v>
+        <v>5.78</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>4.93</v>
       </c>
       <c r="E32">
-        <v>2.67</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C33">
-        <v>5.78</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>4.93</v>
+        <v>2.67</v>
       </c>
       <c r="E33">
-        <v>3.53</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>6.49</v>
       </c>
       <c r="D34">
-        <v>2.67</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>1.07</v>
+        <v>30.43</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C35">
-        <v>6.49</v>
+        <v>2.61</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>30.43</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C36">
-        <v>2.61</v>
+        <v>0.22</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>2.73</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C37">
-        <v>0.22</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="E37">
-        <v>0.23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C38">
-        <v>2.2799999999999998</v>
+        <v>37.08</v>
       </c>
       <c r="D38">
-        <v>2.4700000000000002</v>
+        <v>28.33</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C39">
-        <v>37.08</v>
+        <v>59.07</v>
       </c>
       <c r="D39">
-        <v>28.33</v>
+        <v>40.4</v>
       </c>
       <c r="E39">
-        <v>44</v>
+        <v>87.67</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40">
-        <v>59.07</v>
-      </c>
-      <c r="D40">
-        <v>40.4</v>
-      </c>
-      <c r="E40">
-        <v>87.67</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>0.04</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C42">
-        <v>0.04</v>
+        <v>1.06</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C43">
-        <v>1.06</v>
+        <v>3.92</v>
       </c>
       <c r="D43">
-        <v>0.73</v>
+        <v>3</v>
       </c>
       <c r="E43">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C44">
         <v>3.92</v>
@@ -1286,13 +1328,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C45">
-        <v>3.92</v>
+        <v>0.47</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>2.17</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1300,1271 +1342,1258 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C46">
-        <v>0.47</v>
+        <v>0.04</v>
       </c>
       <c r="D46">
-        <v>2.17</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C47">
-        <v>0.04</v>
+        <v>9.92</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>10.9</v>
       </c>
       <c r="E47">
-        <v>0.33</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48">
-        <v>9.92</v>
-      </c>
-      <c r="D48">
-        <v>10.9</v>
-      </c>
-      <c r="E48">
-        <v>1.42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="C49">
+        <v>33.82</v>
+      </c>
+      <c r="D49">
+        <v>31.22</v>
+      </c>
+      <c r="E49">
+        <v>34.659999999999997</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C50">
-        <v>33.82</v>
+        <v>16.09</v>
       </c>
       <c r="D50">
-        <v>31.22</v>
+        <v>16.03</v>
       </c>
       <c r="E50">
-        <v>34.659999999999997</v>
+        <v>13.22</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C51">
-        <v>16.09</v>
+        <v>23.61</v>
       </c>
       <c r="D51">
-        <v>16.03</v>
+        <v>23.7</v>
       </c>
       <c r="E51">
-        <v>13.22</v>
+        <v>16.420000000000002</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52">
-        <v>23.61</v>
-      </c>
-      <c r="D52">
-        <v>23.7</v>
-      </c>
-      <c r="E52">
-        <v>16.420000000000002</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="C53" s="2">
+        <v>105236</v>
+      </c>
+      <c r="D53" s="2">
+        <v>81443</v>
+      </c>
+      <c r="E53" s="2">
+        <v>90971</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C54" s="2">
-        <v>105236</v>
+        <v>7069</v>
       </c>
       <c r="D54" s="2">
-        <v>81443</v>
-      </c>
-      <c r="E54" s="2">
-        <v>90971</v>
+        <v>3777</v>
+      </c>
+      <c r="E54" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C55" s="2">
-        <v>7069</v>
-      </c>
-      <c r="D55" s="2">
-        <v>3777</v>
+        <v>68107</v>
+      </c>
+      <c r="D55" t="s">
+        <v>50</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="2">
-        <v>68107</v>
-      </c>
-      <c r="D56" t="s">
-        <v>53</v>
-      </c>
-      <c r="E56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="C57" s="2">
+        <v>57319</v>
+      </c>
+      <c r="D57" s="2">
+        <v>79603</v>
+      </c>
+      <c r="E57" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C58" s="2">
-        <v>57319</v>
-      </c>
-      <c r="D58" s="2">
-        <v>79603</v>
+        <v>58039</v>
+      </c>
+      <c r="D58" t="s">
+        <v>50</v>
       </c>
       <c r="E58" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C59" s="2">
-        <v>58039</v>
+        <v>79300</v>
       </c>
       <c r="D59" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E59" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C60" s="2">
-        <v>79300</v>
+        <v>32326</v>
       </c>
       <c r="D60" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E60" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>59</v>
-      </c>
-      <c r="C61" s="2">
-        <v>32326</v>
+        <v>57</v>
+      </c>
+      <c r="C61" t="s">
+        <v>50</v>
       </c>
       <c r="D61" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E61" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>60</v>
-      </c>
-      <c r="C62" t="s">
-        <v>53</v>
-      </c>
-      <c r="D62" t="s">
-        <v>53</v>
-      </c>
-      <c r="E62" t="s">
-        <v>53</v>
+        <v>10</v>
+      </c>
+      <c r="C62" s="2">
+        <v>73</v>
+      </c>
+      <c r="D62" s="2">
+        <v>73</v>
+      </c>
+      <c r="E62" s="2">
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="2">
-        <v>73</v>
-      </c>
-      <c r="D63" s="2">
-        <v>73</v>
-      </c>
-      <c r="E63" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>10</v>
+      </c>
+      <c r="C66" s="2">
+        <v>73</v>
+      </c>
+      <c r="D66" s="2">
+        <v>73</v>
+      </c>
+      <c r="E66" s="2">
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C67" s="2">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="D67" s="2">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E67" s="2">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C68" s="2">
-        <v>51</v>
+        <v>173</v>
       </c>
       <c r="D68" s="2">
-        <v>53</v>
+        <v>317</v>
       </c>
       <c r="E68" s="2">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C69" s="2">
-        <v>173</v>
+        <v>216</v>
       </c>
       <c r="D69" s="2">
-        <v>317</v>
+        <v>180</v>
       </c>
       <c r="E69" s="2">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C70" s="2">
-        <v>216</v>
+        <v>1085</v>
       </c>
       <c r="D70" s="2">
-        <v>180</v>
+        <v>808</v>
       </c>
       <c r="E70" s="2">
-        <v>107</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C71" s="2">
-        <v>1085</v>
+        <v>213</v>
       </c>
       <c r="D71" s="2">
-        <v>808</v>
+        <v>270</v>
       </c>
       <c r="E71" s="2">
-        <v>1757</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C72" s="2">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="D72" s="2">
-        <v>270</v>
+        <v>49</v>
       </c>
       <c r="E72" s="2">
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C73" s="2">
-        <v>237</v>
+        <v>788</v>
       </c>
       <c r="D73" s="2">
-        <v>49</v>
+        <v>812</v>
       </c>
       <c r="E73" s="2">
-        <v>0</v>
+        <v>719</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C74" s="2">
-        <v>788</v>
+        <v>507</v>
       </c>
       <c r="D74" s="2">
-        <v>812</v>
+        <v>148</v>
       </c>
       <c r="E74" s="2">
-        <v>719</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C75" s="2">
-        <v>507</v>
+        <v>385</v>
       </c>
       <c r="D75" s="2">
-        <v>148</v>
+        <v>336</v>
       </c>
       <c r="E75" s="2">
-        <v>71</v>
+        <v>307</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C76" s="2">
-        <v>385</v>
+        <v>98</v>
       </c>
       <c r="D76" s="2">
-        <v>336</v>
+        <v>171</v>
       </c>
       <c r="E76" s="2">
-        <v>307</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C77" s="2">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="D77" s="2">
-        <v>171</v>
+        <v>290</v>
       </c>
       <c r="E77" s="2">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C78" s="2">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="D78" s="2">
-        <v>290</v>
+        <v>75</v>
       </c>
       <c r="E78" s="2">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C79" s="2">
-        <v>190</v>
+        <v>45</v>
       </c>
       <c r="D79" s="2">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="E79" s="2">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C80" s="2">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D80" s="2">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E80" s="2">
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C81" s="2">
-        <v>32</v>
+        <v>1007</v>
       </c>
       <c r="D81" s="2">
-        <v>15</v>
+        <v>2234</v>
       </c>
       <c r="E81" s="2">
-        <v>19</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C82" s="2">
-        <v>1007</v>
+        <v>418</v>
       </c>
       <c r="D82" s="2">
-        <v>2234</v>
+        <v>637</v>
       </c>
       <c r="E82" s="2">
-        <v>185</v>
+        <v>260</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C83" s="2">
-        <v>418</v>
+        <v>946</v>
       </c>
       <c r="D83" s="2">
-        <v>637</v>
+        <v>1349</v>
       </c>
       <c r="E83" s="2">
-        <v>260</v>
+        <v>835</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C84" s="2">
-        <v>946</v>
+        <v>6627</v>
       </c>
       <c r="D84" s="2">
-        <v>1349</v>
+        <v>7805</v>
       </c>
       <c r="E84" s="2">
-        <v>835</v>
+        <v>4719</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>63</v>
-      </c>
-      <c r="C85" s="2">
-        <v>6627</v>
-      </c>
-      <c r="D85" s="2">
-        <v>7805</v>
-      </c>
-      <c r="E85" s="2">
-        <v>4719</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>64</v>
+        <v>10</v>
+      </c>
+      <c r="C86" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D86" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E86" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C87" s="3">
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="D87" s="3">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E87" s="3">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C88" s="3">
-        <v>0.18</v>
+        <v>0.6</v>
       </c>
       <c r="D88" s="3">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="E88" s="3">
-        <v>0.12</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C89" s="3">
-        <v>0.6</v>
+        <v>0.76</v>
       </c>
       <c r="D89" s="3">
-        <v>0.85</v>
+        <v>0.51</v>
       </c>
       <c r="E89" s="3">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C90" s="3">
-        <v>0.76</v>
+        <v>3.98</v>
       </c>
       <c r="D90" s="3">
-        <v>0.51</v>
+        <v>2.16</v>
       </c>
       <c r="E90" s="3">
-        <v>0.44</v>
+        <v>7.58</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C91" s="3">
-        <v>3.98</v>
+        <v>0.73</v>
       </c>
       <c r="D91" s="3">
-        <v>2.16</v>
+        <v>0.76</v>
       </c>
       <c r="E91" s="3">
-        <v>7.58</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C92" s="3">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
       <c r="D92" s="3">
-        <v>0.76</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E92" s="3">
-        <v>0.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C93" s="3">
-        <v>0.85</v>
+        <v>2.81</v>
       </c>
       <c r="D93" s="3">
-        <v>0.14000000000000001</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="E93" s="3">
-        <v>0</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C94" s="3">
-        <v>2.81</v>
+        <v>1.81</v>
       </c>
       <c r="D94" s="3">
-        <v>2.2599999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="E94" s="3">
-        <v>3.02</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C95" s="3">
-        <v>1.81</v>
+        <v>1.37</v>
       </c>
       <c r="D95" s="3">
-        <v>0.4</v>
+        <v>0.96</v>
       </c>
       <c r="E95" s="3">
-        <v>0.33</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C96" s="3">
-        <v>1.37</v>
+        <v>0.34</v>
       </c>
       <c r="D96" s="3">
-        <v>0.96</v>
+        <v>0.48</v>
       </c>
       <c r="E96" s="3">
-        <v>1.25</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C97" s="3">
-        <v>0.34</v>
+        <v>0.59</v>
       </c>
       <c r="D97" s="3">
-        <v>0.48</v>
+        <v>0.8</v>
       </c>
       <c r="E97" s="3">
-        <v>0.34</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C98" s="3">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="D98" s="3">
-        <v>0.8</v>
+        <v>0.21</v>
       </c>
       <c r="E98" s="3">
-        <v>0.32</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C99" s="3">
-        <v>0.67</v>
+        <v>0.17</v>
       </c>
       <c r="D99" s="3">
-        <v>0.21</v>
+        <v>0.09</v>
       </c>
       <c r="E99" s="3">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C100" s="3">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
       <c r="D100" s="3">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
       <c r="E100" s="3">
-        <v>0.22</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C101" s="3">
-        <v>0.12</v>
+        <v>3.39</v>
       </c>
       <c r="D101" s="3">
-        <v>0.04</v>
+        <v>6.29</v>
       </c>
       <c r="E101" s="3">
-        <v>0.08</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C102" s="3">
-        <v>3.39</v>
+        <v>1.4</v>
       </c>
       <c r="D102" s="3">
-        <v>6.29</v>
+        <v>1.7</v>
       </c>
       <c r="E102" s="3">
-        <v>0.78</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C103" s="3">
-        <v>1.4</v>
+        <v>3.31</v>
       </c>
       <c r="D103" s="3">
-        <v>1.7</v>
+        <v>3.92</v>
       </c>
       <c r="E103" s="3">
-        <v>1.03</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C104" s="3">
-        <v>3.31</v>
+        <v>23.32</v>
       </c>
       <c r="D104" s="3">
-        <v>3.92</v>
+        <v>21.8</v>
       </c>
       <c r="E104" s="3">
-        <v>3.48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C105" s="3">
-        <v>23.32</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D105" s="3">
-        <v>21.8</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="E105" s="3">
-        <v>20</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C106" s="3">
-        <v>2.2999999999999998</v>
+        <v>4.62</v>
       </c>
       <c r="D106" s="3">
-        <v>2.2400000000000002</v>
+        <v>2.66</v>
       </c>
       <c r="E106" s="3">
-        <v>1.91</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C107" s="3">
-        <v>4.62</v>
+        <v>3.39</v>
       </c>
       <c r="D107" s="3">
-        <v>2.66</v>
+        <v>6.29</v>
       </c>
       <c r="E107" s="3">
-        <v>3.35</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C108" s="3">
-        <v>3.39</v>
+        <v>5.55</v>
       </c>
       <c r="D108" s="3">
-        <v>6.29</v>
+        <v>3.22</v>
       </c>
       <c r="E108" s="3">
-        <v>0.78</v>
+        <v>8.2899999999999991</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>68</v>
-      </c>
-      <c r="C109" s="3">
-        <v>5.55</v>
-      </c>
-      <c r="D109" s="3">
-        <v>3.22</v>
-      </c>
-      <c r="E109" s="3">
-        <v>8.2899999999999991</v>
+        <v>66</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="C110" s="3">
+        <v>12.82</v>
+      </c>
+      <c r="D110" s="3">
+        <v>6.57</v>
+      </c>
+      <c r="E110" s="3">
+        <v>19.62</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C111" s="3">
-        <v>12.82</v>
+        <v>1.85</v>
       </c>
       <c r="D111" s="3">
-        <v>6.57</v>
+        <v>1.51</v>
       </c>
       <c r="E111" s="3">
-        <v>19.62</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C112" s="3">
-        <v>1.85</v>
+        <v>6.38</v>
       </c>
       <c r="D112" s="3">
-        <v>1.51</v>
+        <v>4.29</v>
       </c>
       <c r="E112" s="3">
-        <v>1.58</v>
+        <v>7.58</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C113" s="3">
-        <v>6.38</v>
+        <v>1.91</v>
       </c>
       <c r="D113" s="3">
-        <v>4.29</v>
+        <v>2.14</v>
       </c>
       <c r="E113" s="3">
-        <v>7.58</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>73</v>
-      </c>
-      <c r="C114" s="3">
-        <v>1.91</v>
-      </c>
-      <c r="D114" s="3">
-        <v>2.14</v>
-      </c>
-      <c r="E114" s="3">
-        <v>1.65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="C115" s="2">
+        <v>12232</v>
+      </c>
+      <c r="D115" s="2">
+        <v>15380</v>
+      </c>
+      <c r="E115" s="2">
+        <v>10750</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C116" s="2">
-        <v>12232</v>
+        <v>43</v>
       </c>
       <c r="D116" s="2">
-        <v>15380</v>
+        <v>43</v>
       </c>
       <c r="E116" s="2">
-        <v>10750</v>
+        <v>46</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>76</v>
-      </c>
-      <c r="C117" s="2">
-        <v>43</v>
-      </c>
-      <c r="D117" s="2">
-        <v>43</v>
-      </c>
-      <c r="E117" s="2">
-        <v>46</v>
+        <v>74</v>
+      </c>
+      <c r="C117" s="1">
+        <v>0.79720000000000002</v>
+      </c>
+      <c r="D117" s="1">
+        <v>0.96450000000000002</v>
+      </c>
+      <c r="E117" s="1">
+        <v>0.64610000000000001</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>77</v>
-      </c>
-      <c r="C118" s="1">
-        <v>0.79720000000000002</v>
-      </c>
-      <c r="D118" s="1">
-        <v>0.96450000000000002</v>
-      </c>
-      <c r="E118" s="1">
-        <v>0.64610000000000001</v>
+        <v>75</v>
+      </c>
+      <c r="C118" s="2">
+        <v>21</v>
+      </c>
+      <c r="D118" s="2">
+        <v>21</v>
+      </c>
+      <c r="E118" s="2">
+        <v>26</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>78</v>
-      </c>
-      <c r="C119" s="2">
-        <v>21</v>
-      </c>
-      <c r="D119" s="2">
-        <v>21</v>
-      </c>
-      <c r="E119" s="2">
-        <v>26</v>
+        <v>76</v>
+      </c>
+      <c r="C119" s="3">
+        <v>12.65</v>
+      </c>
+      <c r="D119" s="3">
+        <v>6.57</v>
+      </c>
+      <c r="E119" s="3">
+        <v>19.62</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>79</v>
-      </c>
-      <c r="C120" s="3">
-        <v>12.65</v>
-      </c>
-      <c r="D120" s="3">
-        <v>6.57</v>
-      </c>
-      <c r="E120" s="3">
-        <v>19.62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>80</v>
+        <v>30</v>
+      </c>
+      <c r="C121">
+        <v>385</v>
+      </c>
+      <c r="D121">
+        <v>491</v>
+      </c>
+      <c r="E121">
+        <v>413</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="C122">
-        <v>385</v>
-      </c>
-      <c r="D122">
-        <v>491</v>
-      </c>
-      <c r="E122">
-        <v>413</v>
+        <v>12</v>
+      </c>
+      <c r="D122" t="s">
+        <v>50</v>
+      </c>
+      <c r="E122" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>81</v>
-      </c>
-      <c r="C123">
-        <v>12</v>
-      </c>
-      <c r="D123" t="s">
-        <v>53</v>
-      </c>
-      <c r="E123" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="C124">
+        <v>0.09</v>
+      </c>
+      <c r="D124">
+        <v>0.11</v>
+      </c>
+      <c r="E124">
+        <v>0.05</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C125">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="D125">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="E125">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>29.4</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>15.06</v>
       </c>
       <c r="E126">
-        <v>0</v>
+        <v>34.93</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>85</v>
-      </c>
-      <c r="C127">
-        <v>29.4</v>
-      </c>
-      <c r="D127">
-        <v>15.06</v>
-      </c>
-      <c r="E127">
-        <v>34.93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="C128" s="1">
+        <v>0.50209999999999999</v>
+      </c>
+      <c r="D128" s="1">
+        <v>0.2833</v>
+      </c>
+      <c r="E128" s="1">
+        <v>0.66</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C129" s="1">
-        <v>0.50209999999999999</v>
+        <v>0.17680000000000001</v>
       </c>
       <c r="D129" s="1">
-        <v>0.2833</v>
+        <v>0.38329999999999997</v>
       </c>
       <c r="E129" s="1">
-        <v>0.66</v>
+        <v>6.7000000000000002E-3</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C130" s="1">
-        <v>0.17680000000000001</v>
+        <v>0.3211</v>
       </c>
       <c r="D130" s="1">
-        <v>0.38329999999999997</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="E130" s="1">
-        <v>6.7000000000000002E-3</v>
+        <v>0.33329999999999999</v>
       </c>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>89</v>
-      </c>
-      <c r="C131" s="1">
-        <v>0.3211</v>
-      </c>
-      <c r="D131" s="1">
-        <v>0.33329999999999999</v>
-      </c>
-      <c r="E131" s="1">
-        <v>0.33329999999999999</v>
+        <v>87</v>
       </c>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0.62450000000000006</v>
+      </c>
+      <c r="D132" s="1">
+        <v>0.2833</v>
+      </c>
+      <c r="E132" s="1">
+        <v>0.74329999999999996</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C133" s="1">
-        <v>0.62450000000000006</v>
+        <v>0.3755</v>
       </c>
       <c r="D133" s="1">
-        <v>0.2833</v>
+        <v>0.7167</v>
       </c>
       <c r="E133" s="1">
-        <v>0.74329999999999996</v>
+        <v>0.25669999999999998</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>92</v>
-      </c>
-      <c r="C134" s="1">
-        <v>0.3755</v>
-      </c>
-      <c r="D134" s="1">
-        <v>0.7167</v>
-      </c>
-      <c r="E134" s="1">
-        <v>0.25669999999999998</v>
+        <v>90</v>
       </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="C135" s="1">
+        <v>0.12640000000000001</v>
+      </c>
+      <c r="D135" s="1">
+        <v>8.6699999999999999E-2</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C136" s="1">
-        <v>0.12640000000000001</v>
+        <v>0.87360000000000004</v>
       </c>
       <c r="D136" s="1">
-        <v>8.6699999999999999E-2</v>
+        <v>0.9133</v>
       </c>
       <c r="E136" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>95</v>
-      </c>
-      <c r="C137" s="1">
-        <v>0.87360000000000004</v>
-      </c>
-      <c r="D137" s="1">
-        <v>0.9133</v>
-      </c>
-      <c r="E137" s="1">
-        <v>1</v>
+        <v>93</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="C138" s="1">
+        <v>0.15509999999999999</v>
+      </c>
+      <c r="D138" s="1">
+        <v>0.45329999999999998</v>
+      </c>
+      <c r="E138" s="1">
+        <v>4.7199999999999999E-2</v>
       </c>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C139" s="1">
-        <v>0.15509999999999999</v>
+        <v>0.13070000000000001</v>
       </c>
       <c r="D139" s="1">
-        <v>0.45329999999999998</v>
+        <v>0.27</v>
       </c>
       <c r="E139" s="1">
-        <v>4.7199999999999999E-2</v>
+        <v>0.1867</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C140" s="1">
-        <v>0.13070000000000001</v>
+        <v>0.51959999999999995</v>
       </c>
       <c r="D140" s="1">
-        <v>0.27</v>
+        <v>0</v>
       </c>
       <c r="E140" s="1">
-        <v>0.1867</v>
+        <v>0.74070000000000003</v>
       </c>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C141" s="1">
-        <v>0.51959999999999995</v>
+        <v>0.19439999999999999</v>
       </c>
       <c r="D141" s="1">
-        <v>0</v>
+        <v>0.2767</v>
       </c>
       <c r="E141" s="1">
-        <v>0.74070000000000003</v>
+        <v>2.3300000000000001E-2</v>
       </c>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C142" s="1">
-        <v>0.19439999999999999</v>
+        <v>4.1700000000000001E-2</v>
       </c>
       <c r="D142" s="1">
-        <v>0.2767</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="E142" s="1">
-        <v>2.3300000000000001E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>101</v>
-      </c>
-      <c r="C143" s="1">
-        <v>4.1700000000000001E-2</v>
-      </c>
-      <c r="D143" s="1">
-        <v>0.33329999999999999</v>
-      </c>
-      <c r="E143" s="1">
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="C144" s="1">
+        <v>0.73029999999999995</v>
+      </c>
+      <c r="D144" s="1">
+        <v>0.40329999999999999</v>
+      </c>
+      <c r="E144" s="1">
+        <v>0.94569999999999999</v>
       </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C145" s="1">
-        <v>0.73029999999999995</v>
+        <v>0.26979999999999998</v>
       </c>
       <c r="D145" s="1">
-        <v>0.40329999999999999</v>
+        <v>0.59670000000000001</v>
       </c>
       <c r="E145" s="1">
-        <v>0.94569999999999999</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5">
-      <c r="A146" t="s">
-        <v>104</v>
-      </c>
-      <c r="C146" s="1">
-        <v>0.26979999999999998</v>
-      </c>
-      <c r="D146" s="1">
-        <v>0.59670000000000001</v>
-      </c>
-      <c r="E146" s="1">
         <v>5.4300000000000001E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>